<commit_message>
alteracao na data da semana de provas
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>Data</t>
   </si>
@@ -136,6 +136,15 @@
     <t>22-Mar</t>
   </si>
   <si>
+    <t>SEMANA DE PROVAS</t>
+  </si>
+  <si>
+    <t>27-Mar</t>
+  </si>
+  <si>
+    <t>29-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
   </si>
   <si>
@@ -148,7 +157,7 @@
     <t>Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>27-Mar</t>
+    <t>03-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
@@ -163,15 +172,6 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>29-Mar</t>
-  </si>
-  <si>
-    <t>SEMANA DE PROVAS</t>
-  </si>
-  <si>
-    <t>03-Abr</t>
-  </si>
-  <si>
     <t>05-Abr</t>
   </si>
   <si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>17-Mai</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -270,7 +267,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,8 +282,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Roboto"/>
       <family val="2"/>
     </font>
@@ -318,34 +321,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,33 +649,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="65.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="85.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="120.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="65.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="85.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="120.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="41.25" customFormat="1" s="3">
+      <c r="F1" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -697,9 +691,9 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F2" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="53.25" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -715,9 +709,9 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="30" customFormat="1" s="3">
+      <c r="F3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -733,9 +727,9 @@
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="30" customFormat="1" s="3">
+      <c r="F4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -751,9 +745,9 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="53.25" customFormat="1" s="1">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -769,9 +763,9 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -787,11 +781,11 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="53.25" customFormat="1" s="3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -807,9 +801,9 @@
       <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F8" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -825,9 +819,9 @@
       <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F9" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -843,9 +837,9 @@
       <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="53.25" customFormat="1" s="3">
+      <c r="F10" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="53.25" customFormat="1" s="1">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -861,9 +855,9 @@
       <c r="E11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="41.25" customFormat="1" s="3">
+      <c r="F11" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -879,117 +873,117 @@
       <c r="E12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="41.25" customFormat="1" s="3">
+      <c r="F12" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="41.25" customFormat="1" s="1">
+      <c r="A14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="41.25" customFormat="1" s="3">
-      <c r="A14" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="F15" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18" customFormat="1" s="3">
-      <c r="A15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18" customFormat="1" s="3">
-      <c r="A16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="41.25" customFormat="1" s="3">
+      <c r="F16" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A17" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="41.25" customFormat="1" s="3">
+        <v>51</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="41.25" customFormat="1" s="3">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="41.25" customFormat="1" s="1">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
@@ -1003,11 +997,11 @@
         <v>57</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18" customFormat="1" s="3">
+        <v>51</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -1023,9 +1017,9 @@
       <c r="E20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F20" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -1041,9 +1035,9 @@
       <c r="E21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F21" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A22" s="5" t="s">
         <v>68</v>
       </c>
@@ -1059,9 +1053,9 @@
       <c r="E22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F22" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A23" s="5" t="s">
         <v>70</v>
       </c>
@@ -1077,27 +1071,27 @@
       <c r="E23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
-      <c r="A24" s="1" t="s">
+      <c r="F23" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F24" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A25" s="5" t="s">
         <v>74</v>
       </c>
@@ -1113,9 +1107,9 @@
       <c r="E25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F25" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1131,9 +1125,9 @@
       <c r="E26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F26" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A27" s="5" t="s">
         <v>79</v>
       </c>
@@ -1149,137 +1143,107 @@
       <c r="E27" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18" customFormat="1" s="3">
+      <c r="F27" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A28" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18" customFormat="1" s="3">
+        <v>40</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A29" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18" customFormat="1" s="3">
-      <c r="A30" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18" customFormat="1" s="3">
-      <c r="A31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18" customFormat="1" s="3">
-      <c r="A32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18" customFormat="1" s="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
alterando plano de aula e critério de avaliação
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Data</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve"> Programação/Atividades </t>
   </si>
   <si>
-    <t>14-Ago</t>
+    <t>05-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Apresentação da disciplina. O que é Inteligência Artificial e qual a sua relação com agente autônomo? </t>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referência: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>16-Ago</t>
+    <t>07-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">O que é agente autônomo? O que são propriedades de ambiente e como isto impacta o desenvolvimento de agentes autônomos? </t>
@@ -57,7 +57,16 @@
     <t xml:space="preserve">Dinâmica em grupo. Referências: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>21-Ago</t>
+    <t>12-Fev</t>
+  </si>
+  <si>
+    <t>Carnaval</t>
+  </si>
+  <si>
+    <t>14-Fev</t>
+  </si>
+  <si>
+    <t>19-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Como especificar o espaço de busca de um agente? </t>
@@ -72,7 +81,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>23-Ago</t>
+    <t>21-Fev</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? </t>
@@ -84,16 +93,16 @@
     <t xml:space="preserve"> Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>28-Ago</t>
-  </si>
-  <si>
-    <t>30-Ago</t>
+    <t>26-Fev</t>
+  </si>
+  <si>
+    <t>28-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>04-Set</t>
+    <t>4-Março</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística?</t>
@@ -105,16 +114,10 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>06-Set</t>
-  </si>
-  <si>
-    <t>11-Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística? </t>
-  </si>
-  <si>
-    <t>13-Set</t>
+    <t>6-Março</t>
+  </si>
+  <si>
+    <t>11-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
@@ -129,13 +132,10 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>18-Set</t>
-  </si>
-  <si>
-    <t>20-Set</t>
-  </si>
-  <si>
-    <t>25-Set</t>
+    <t>13-Março</t>
+  </si>
+  <si>
+    <t>18-Março</t>
   </si>
   <si>
     <t xml:space="preserve">SEMANA DE PROVAS</t>
@@ -144,13 +144,13 @@
     <t xml:space="preserve">SEMANA DE PROVAS - Prova Intermediária</t>
   </si>
   <si>
-    <t>27-Set</t>
+    <t>20-Março</t>
   </si>
   <si>
     <t xml:space="preserve">SEMANA DE PROVAS - Não teremos aula</t>
   </si>
   <si>
-    <t>02-Out</t>
+    <t>25-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>04-Out</t>
+    <t>27-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
@@ -180,13 +180,13 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>09-Out</t>
-  </si>
-  <si>
-    <t>11-Out</t>
-  </si>
-  <si>
-    <t>16-Out</t>
+    <t>1-Abril</t>
+  </si>
+  <si>
+    <t>3-Abril</t>
+  </si>
+  <si>
+    <t>8-Abril</t>
   </si>
   <si>
     <t xml:space="preserve">O que é aprendizagem por reforço? Qual a sua relação com o desenvolvimento de agentes autônomos? </t>
@@ -198,7 +198,7 @@
     <t xml:space="preserve"> Discussão em sala. </t>
   </si>
   <si>
-    <t>18-Out</t>
+    <t>10-Abril</t>
   </si>
   <si>
     <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
@@ -213,7 +213,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>23-Out</t>
+    <t>15-Abril</t>
   </si>
   <si>
     <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
@@ -228,16 +228,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>25-Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quais são os limites e detalhes do algoritmo Q-Learning? </t>
-  </si>
-  <si>
-    <t>30-Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Não teremos aula</t>
+    <t>17-Abril</t>
   </si>
   <si>
     <t xml:space="preserve">Reinforcement Learning: métodos tabulares</t>
@@ -246,19 +237,46 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t xml:space="preserve">Sem Aula - Semana de Provas</t>
+    <t>22-Abril</t>
+  </si>
+  <si>
+    <t>24-Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento de um agente robótico (físico).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de um projeto envolvendo um kit de robótica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento de projeto</t>
+  </si>
+  <si>
+    <t>29-Abril</t>
+  </si>
+  <si>
+    <t>01-Maio</t>
+  </si>
+  <si>
+    <t>Feriado</t>
+  </si>
+  <si>
+    <t>6-Maio</t>
+  </si>
+  <si>
+    <t>8-Maio</t>
+  </si>
+  <si>
+    <t>13-Maio</t>
   </si>
   <si>
     <t xml:space="preserve">Avaliação Final da disciplina</t>
   </si>
   <si>
-    <t>22-Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula de fechamento com entrega de projeto e avaliação</t>
-  </si>
-  <si>
-    <t/>
+    <t>15-Maio</t>
   </si>
 </sst>
 </file>
@@ -303,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -323,14 +341,17 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,7 +914,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" s="3" customFormat="1" ht="63.75" customHeight="1">
+    <row r="3" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -911,226 +932,226 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" s="3" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" s="3" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" s="3" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" s="3" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A11" s="6" t="s">
+    <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1148,7 +1169,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1263,10 +1284,10 @@
         <v>72</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>70</v>
@@ -1275,144 +1296,162 @@
     </row>
     <row r="24" s="3" customFormat="1" ht="37.5" customHeight="1">
       <c r="A24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="8">
-        <v>45231</v>
+    <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>70</v>
+      <c r="C25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="8">
-        <v>45236</v>
+      <c r="A26" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>70</v>
+      <c r="C26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="8">
-        <v>45238</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A28" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="8">
-        <v>45243</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="A30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+    <row r="31" s="3" customFormat="1" ht="39" customHeight="1">
+      <c r="A31" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1439,6 +1478,22 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
+    <row r="37" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
detalhes plano de aula e primeiras aulas do semestre
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,11 +13,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Data</t>
   </si>
   <si>
+    <t>Tópico</t>
+  </si>
+  <si>
     <t>Questão/Problema/Desafio</t>
   </si>
   <si>
@@ -33,6 +36,9 @@
     <t>05-Fev</t>
   </si>
   <si>
+    <t xml:space="preserve">Introdução à Inteligência Artificial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Apresentação da disciplina. O que é Inteligência Artificial e qual a sua relação com agente autônomo? </t>
   </si>
   <si>
@@ -60,7 +66,7 @@
     <t>12-Fev</t>
   </si>
   <si>
-    <t>Carnaval</t>
+    <t>&lt;strong&gt;Carnaval&lt;/strong&gt;</t>
   </si>
   <si>
     <t>14-Fev</t>
@@ -69,6 +75,9 @@
     <t>19-Fev</t>
   </si>
   <si>
+    <t xml:space="preserve">Algoritmos de busca cegos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como especificar o espaço de busca de um agente? </t>
   </si>
   <si>
@@ -105,6 +114,9 @@
     <t>4-Março</t>
   </si>
   <si>
+    <t xml:space="preserve">Algoritmos de busca informados</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística?</t>
   </si>
   <si>
@@ -120,6 +132,9 @@
     <t>11-Março</t>
   </si>
   <si>
+    <t>13-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
   </si>
   <si>
@@ -132,42 +147,42 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>13-Março</t>
-  </si>
-  <si>
     <t>18-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">SEMANA DE PROVAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEMANA DE PROVAS - Prova Intermediária</t>
-  </si>
-  <si>
     <t>20-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">SEMANA DE PROVAS - Não teremos aula</t>
+    <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Satisfaction Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de um agente autônomo capaz de identificar estados que satisfazem determinadas restrições.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
     <t>25-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Satisfaction Problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de um agente autônomo capaz de identificar estados que satisfazem determinadas restrições.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
   </si>
   <si>
     <t>27-Março</t>
   </si>
   <si>
+    <t>1-Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambientes competitivos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
   </si>
   <si>
@@ -180,15 +195,18 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>1-Abril</t>
-  </si>
-  <si>
     <t>3-Abril</t>
   </si>
   <si>
     <t>8-Abril</t>
   </si>
   <si>
+    <t>10-Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aprendendo políticas</t>
+  </si>
+  <si>
     <t xml:space="preserve">O que é aprendizagem por reforço? Qual a sua relação com o desenvolvimento de agentes autônomos? </t>
   </si>
   <si>
@@ -198,7 +216,7 @@
     <t xml:space="preserve"> Discussão em sala. </t>
   </si>
   <si>
-    <t>10-Abril</t>
+    <t>15-Abril</t>
   </si>
   <si>
     <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
@@ -213,7 +231,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>15-Abril</t>
+    <t>17-Abril</t>
   </si>
   <si>
     <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
@@ -228,7 +246,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>17-Abril</t>
+    <t>22-Abril</t>
   </si>
   <si>
     <t xml:space="preserve">Reinforcement Learning: métodos tabulares</t>
@@ -237,12 +255,12 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>22-Abril</t>
-  </si>
-  <si>
     <t>24-Abril</t>
   </si>
   <si>
+    <t>Robótica</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
   </si>
   <si>
@@ -261,7 +279,7 @@
     <t>01-Maio</t>
   </si>
   <si>
-    <t>Feriado</t>
+    <t>&lt;strong&gt;Feriado&lt;/strong&gt;</t>
   </si>
   <si>
     <t>6-Maio</t>
@@ -273,7 +291,7 @@
     <t>13-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Avaliação Final da disciplina</t>
+    <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
   </si>
   <si>
     <t>15-Maio</t>
@@ -292,12 +310,10 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.000000"/>
-      <color indexed="64"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -321,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -346,12 +362,6 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,25 +874,26 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E16" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="19.147857142857141"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="2" width="38.862142857142857"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="2" width="65.290714285714287"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="2" width="85.719285714285704"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="120.7192857142857"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="2" width="13.005000000000001"/>
+    <col customWidth="1" min="2" max="2" style="1" width="19.147857142857141"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="2" width="38.862142857142857"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="2" width="65.290714285714287"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="85.719285714285704"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" style="2" width="120.7192857142857"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" style="2" width="13.005000000000001"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -894,377 +905,408 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="34.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>28</v>
+      <c r="G9" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" s="3" customFormat="1" ht="20.25" customHeight="1">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" s="3" customFormat="1" ht="49.5" customHeight="1">
       <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="F14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" s="3" customFormat="1" ht="60.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" s="3" customFormat="1" ht="48.75" customHeight="1">
+        <v>45</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" s="3" customFormat="1" ht="48.75" customHeight="1">
+        <v>50</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="5" t="s">
         <v>62</v>
       </c>
+      <c r="B21" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="C21" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" s="3" customFormat="1" ht="44.25" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
         <v>68</v>
       </c>
@@ -1274,225 +1316,246 @@
       <c r="E22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" s="3" customFormat="1" ht="34.5" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" s="3" customFormat="1" ht="37.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>72</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="5"/>
+      <c r="A25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>77</v>
+      <c r="A26" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="D29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="9" t="s">
+      <c r="E29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="A30" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" s="3" customFormat="1" ht="39" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>86</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B31" s="6"/>
       <c r="C31" s="8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="6"/>
-      <c r="B32" s="8"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
atualizando o plano de aula
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Data</t>
   </si>
@@ -33,7 +33,7 @@
     <t xml:space="preserve"> Programação/Atividades </t>
   </si>
   <si>
-    <t>05-Fev</t>
+    <t>14-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Inteligência Artificial</t>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referência: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>07-Fev</t>
+    <t>19-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">O que é agente autônomo? O que são propriedades de ambiente e como isto impacta o desenvolvimento de agentes autônomos? </t>
@@ -63,16 +63,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referências: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>12-Fev</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Carnaval&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>14-Fev</t>
-  </si>
-  <si>
-    <t>19-Fev</t>
+    <t>21-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca cegos</t>
@@ -90,7 +81,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>21-Fev</t>
+    <t>26-Ago</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? </t>
@@ -102,37 +93,49 @@
     <t xml:space="preserve"> Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>26-Fev</t>
-  </si>
-  <si>
-    <t>28-Fev</t>
+    <t>28-Ago</t>
+  </si>
+  <si>
+    <t>2-Set</t>
+  </si>
+  <si>
+    <t>4-Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algoritmos de busca informados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estratégia de busca. Algoritmos de busca **informados** (busca gananciosa, $A^{*}$, família subida da montanha). Função heurística. Comparação entre os algoritmos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
+  </si>
+  <si>
+    <t>9-Set</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>4-Março</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algoritmos de busca informados</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Estratégia de busca. Algoritmos de busca **informados** (busca gananciosa, $A^{*}$, família subida da montanha). Função heurística. Comparação entre os algoritmos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
-  </si>
-  <si>
-    <t>6-Março</t>
-  </si>
-  <si>
-    <t>11-Março</t>
-  </si>
-  <si>
-    <t>13-Março</t>
+    <t>11-Set</t>
+  </si>
+  <si>
+    <t>16-Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>18-Set</t>
+  </si>
+  <si>
+    <t>23-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
@@ -147,10 +150,10 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>18-Março</t>
-  </si>
-  <si>
-    <t>20-Março</t>
+    <t>25-Set</t>
+  </si>
+  <si>
+    <t>30-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
@@ -165,19 +168,7 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>25-Março</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>27-Março</t>
-  </si>
-  <si>
-    <t>1-Abril</t>
+    <t>2-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Ambientes competitivos</t>
@@ -195,13 +186,13 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>3-Abril</t>
-  </si>
-  <si>
-    <t>8-Abril</t>
-  </si>
-  <si>
-    <t>10-Abril</t>
+    <t>7-Out</t>
+  </si>
+  <si>
+    <t>9-Out</t>
+  </si>
+  <si>
+    <t>14-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Aprendendo políticas</t>
@@ -216,7 +207,7 @@
     <t xml:space="preserve"> Discussão em sala. </t>
   </si>
   <si>
-    <t>15-Abril</t>
+    <t>16-Out</t>
   </si>
   <si>
     <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
@@ -231,7 +222,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>17-Abril</t>
+    <t>21-Out</t>
   </si>
   <si>
     <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
@@ -246,7 +237,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>22-Abril</t>
+    <t>23-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Reinforcement Learning: métodos tabulares</t>
@@ -255,7 +246,7 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>24-Abril</t>
+    <t>29-Out</t>
   </si>
   <si>
     <t>Robótica</t>
@@ -273,28 +264,10 @@
     <t xml:space="preserve">Desenvolvimento de projeto</t>
   </si>
   <si>
-    <t>29-Abril</t>
-  </si>
-  <si>
-    <t>01-Maio</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Feriado&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>6-Maio</t>
-  </si>
-  <si>
-    <t>8-Maio</t>
-  </si>
-  <si>
-    <t>13-Maio</t>
+    <t>30-Out</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>15-Maio</t>
   </si>
 </sst>
 </file>
@@ -337,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -359,6 +332,12 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -874,7 +853,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="E16" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -932,7 +911,7 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4"/>
@@ -951,565 +930,516 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4"/>
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="34.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
+      <c r="A7" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
+      <c r="D11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>24</v>
+      <c r="F12" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="7"/>
+      <c r="A13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" s="3" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" s="3" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="7"/>
+      <c r="A15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
+    <row r="16" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>51</v>
+      <c r="C16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="7" t="s">
+    <row r="17" s="3" customFormat="1" ht="69" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>51</v>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" s="3" customFormat="1" ht="44.25" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>74</v>
+      </c>
       <c r="C22" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" s="3" customFormat="1" ht="34.5" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="C23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" s="3" customFormat="1" ht="37.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>76</v>
+      <c r="D24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8">
+        <v>45600</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="E25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="F25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A26" s="8">
+        <v>45602</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A27" s="8">
+        <v>45607</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>88</v>
+      <c r="E27" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="A28" s="8">
+        <v>45609</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>85</v>
+      <c r="D28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="G28" s="5"/>
     </row>
     <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>92</v>
-      </c>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" s="3" customFormat="1" ht="39" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">

</xml_diff>

<commit_message>
plano de aula revisado
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Data</t>
   </si>
@@ -267,7 +267,19 @@
     <t>30-Out</t>
   </si>
   <si>
+    <t>`4-Nov</t>
+  </si>
+  <si>
+    <t>`6-Nov</t>
+  </si>
+  <si>
+    <t>`11-Nov</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>`13-Nov</t>
   </si>
 </sst>
 </file>
@@ -853,7 +865,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1336,8 +1348,8 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="8">
-        <v>45600</v>
+      <c r="A25" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>79</v>
@@ -1354,8 +1366,8 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="8">
-        <v>45602</v>
+      <c r="A26" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>79</v>
@@ -1372,40 +1384,40 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="8">
-        <v>45607</v>
+      <c r="A27" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="8">
-        <v>45609</v>
+      <c r="A28" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
atualizacao do plano de aula - data de provas
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -126,28 +126,28 @@
     <t>16-Set</t>
   </si>
   <si>
+    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desenvolvimento de um agente autônomo que atua em um ambiente discreto, determinístico, síncrono, simulado e *single agent*. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação de um projeto, provavelmente, envolvendo algum framework de simulação (i.e., Gym Open AI). </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
+  </si>
+  <si>
+    <t>18-Set</t>
+  </si>
+  <si>
+    <t>23-Set</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>18-Set</t>
-  </si>
-  <si>
-    <t>23-Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Desenvolvimento de um agente autônomo que atua em um ambiente discreto, determinístico, síncrono, simulado e *single agent*. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação de um projeto, provavelmente, envolvendo algum framework de simulação (i.e., Gym Open AI). </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
     <t>25-Set</t>
@@ -322,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -344,12 +344,6 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1020,10 +1014,10 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1041,10 +1035,10 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1062,7 +1056,7 @@
       </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1080,85 +1074,85 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="D12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="D13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="F13" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" s="3" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="D14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="F14" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="5" t="s">
         <v>47</v>
       </c>
@@ -1174,7 +1168,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1195,7 +1189,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="69" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="6"/>
@@ -1311,7 +1305,7 @@
       <c r="A23" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1332,7 +1326,7 @@
       <c r="A24" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
         <v>79</v>
       </c>
@@ -1348,7 +1342,7 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1366,7 +1360,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1384,51 +1378,51 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G28" s="5"/>
     </row>
     <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" s="3" customFormat="1" ht="39" customHeight="1">
@@ -1439,19 +1433,19 @@
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">

</xml_diff>

<commit_message>
pre aula dia 02/09
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Data</t>
   </si>
@@ -114,6 +114,9 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
+    <t>5-Set</t>
+  </si>
+  <si>
     <t>9-Set</t>
   </si>
   <si>
@@ -123,24 +126,57 @@
     <t>11-Set</t>
   </si>
   <si>
+    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desenvolvimento de um agente autônomo que atua em um ambiente discreto, determinístico, síncrono, simulado e *single agent*. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação de um projeto, provavelmente, envolvendo algum framework de simulação (i.e., Gym Open AI). </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
+  </si>
+  <si>
+    <t>12-Set</t>
+  </si>
+  <si>
     <t>16-Set</t>
   </si>
   <si>
-    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Desenvolvimento de um agente autônomo que atua em um ambiente discreto, determinístico, síncrono, simulado e *single agent*. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação de um projeto, provavelmente, envolvendo algum framework de simulação (i.e., Gym Open AI). </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
+    <t xml:space="preserve">Ambientes competitivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Satisfaction Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de um agente autônomo capaz de identificar estados que satisfazem determinadas restrições.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
     <t>18-Set</t>
   </si>
   <si>
+    <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jogos de tabuleiro, busca competitiva, algoritmo min-max e função de utilidade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação de um agente autônomo que deverá atuar em um ambiente competitivo, determinístico e completamente observável. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
+  </si>
+  <si>
+    <t>19-Set</t>
+  </si>
+  <si>
     <t>23-Set</t>
   </si>
   <si>
@@ -156,130 +192,103 @@
     <t>30-Set</t>
   </si>
   <si>
-    <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Satisfaction Problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de um agente autônomo capaz de identificar estados que satisfazem determinadas restrições.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
+    <t xml:space="preserve">Aprendendo políticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O que é aprendizagem por reforço? Qual a sua relação com o desenvolvimento de agentes autônomos? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição de aprendizagem por reforço, política de controle e algoritmo Q-Learning. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discussão em sala. </t>
   </si>
   <si>
     <t>2-Out</t>
   </si>
   <si>
-    <t xml:space="preserve">Ambientes competitivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jogos de tabuleiro, busca competitiva, algoritmo min-max e função de utilidade. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação de um agente autônomo que deverá atuar em um ambiente competitivo, determinístico e completamente observável. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
+    <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Apresentação do ambiente OpenAI Gym. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exercícios em sala de aula envolvendo o ambiente OpenAI Gym. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
     <t>7-Out</t>
   </si>
   <si>
+    <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Algoritmo Q-Learning: detalhes e hiperparâmetros. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
+  </si>
+  <si>
     <t>9-Out</t>
   </si>
   <si>
+    <t xml:space="preserve">Reinforcement Learning: métodos tabulares</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
+  </si>
+  <si>
     <t>14-Out</t>
   </si>
   <si>
-    <t xml:space="preserve">Aprendendo políticas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O que é aprendizagem por reforço? Qual a sua relação com o desenvolvimento de agentes autônomos? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definição de aprendizagem por reforço, política de controle e algoritmo Q-Learning. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Discussão em sala. </t>
-  </si>
-  <si>
     <t>16-Out</t>
   </si>
   <si>
-    <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Apresentação do ambiente OpenAI Gym. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exercícios em sala de aula envolvendo o ambiente OpenAI Gym. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
-  </si>
-  <si>
     <t>21-Out</t>
   </si>
   <si>
-    <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Algoritmo Q-Learning: detalhes e hiperparâmetros. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
+    <t>Robótica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento de um agente robótico (físico).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de um projeto envolvendo um kit de robótica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento de projeto</t>
   </si>
   <si>
     <t>23-Out</t>
   </si>
   <si>
-    <t xml:space="preserve">Reinforcement Learning: métodos tabulares</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
-  </si>
-  <si>
     <t>29-Out</t>
   </si>
   <si>
-    <t>Robótica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento de um agente robótico (físico).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação de um projeto envolvendo um kit de robótica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento de projeto</t>
-  </si>
-  <si>
     <t>30-Out</t>
   </si>
   <si>
-    <t>`4-Nov</t>
-  </si>
-  <si>
-    <t>`6-Nov</t>
-  </si>
-  <si>
-    <t>`11-Nov</t>
+    <t>4-Nov</t>
+  </si>
+  <si>
+    <t>6-Nov</t>
+  </si>
+  <si>
+    <t>11-Nov</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>`13-Nov</t>
+    <t>13-Nov</t>
   </si>
 </sst>
 </file>
@@ -322,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -344,6 +353,12 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -859,7 +874,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1035,7 +1050,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="7"/>
@@ -1051,14 +1066,13 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1071,10 +1085,12 @@
       <c r="F10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1089,13 +1105,12 @@
       <c r="F11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
@@ -1108,371 +1123,399 @@
       <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" s="3" customFormat="1" ht="48.75" customHeight="1">
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" s="3" customFormat="1" ht="49.5" customHeight="1">
+      <c r="D13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" s="3" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>46</v>
+      <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" s="3" customFormat="1" ht="63" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="D16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="F16" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" s="3" customFormat="1" ht="69" customHeight="1">
+    <row r="17" s="3" customFormat="1" ht="49.5" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="D17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="F17" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A18" s="6" t="s">
+    <row r="18" s="3" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="B18" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>60</v>
-      </c>
+    <row r="19" s="3" customFormat="1" ht="63" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" s="3" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="6"/>
+    <row r="20" s="3" customFormat="1" ht="69" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" s="3" customFormat="1" ht="44.25" customHeight="1">
+    <row r="22" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" s="3" customFormat="1" ht="34.5" customHeight="1">
+    <row r="23" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" s="3" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" s="3" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="F24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" s="3" customFormat="1" ht="44.25" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" s="3" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" s="3" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" s="3" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8" t="s">
+      <c r="F27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="48" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="C28" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A29" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="C29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G29" s="5"/>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="7"/>
+      <c r="A30" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="B30" s="7"/>
+      <c r="C30" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" s="3" customFormat="1" ht="39" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+    <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+    <row r="34" s="3" customFormat="1" ht="39" customHeight="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1493,6 +1536,33 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
+    <row r="39" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
atualizacao do plano de aula para o semestre 2025_1
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
@@ -9,11 +9,14 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Data</t>
   </si>
@@ -33,7 +36,7 @@
     <t xml:space="preserve"> Programação/Atividades </t>
   </si>
   <si>
-    <t>14-Ago</t>
+    <t>03-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Inteligência Artificial</t>
@@ -51,7 +54,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referência: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>19-Ago</t>
+    <t>05-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">O que é agente autônomo? O que são propriedades de ambiente e como isto impacta o desenvolvimento de agentes autônomos? </t>
@@ -63,7 +66,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referências: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>21-Ago</t>
+    <t>10-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca cegos</t>
@@ -81,7 +84,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>26-Ago</t>
+    <t>12-Fev</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? </t>
@@ -93,13 +96,13 @@
     <t xml:space="preserve"> Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>28-Ago</t>
-  </si>
-  <si>
-    <t>2-Set</t>
-  </si>
-  <si>
-    <t>4-Set</t>
+    <t>17-Fev</t>
+  </si>
+  <si>
+    <t>19-Fev</t>
+  </si>
+  <si>
+    <t>24-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca informados</t>
@@ -114,18 +117,12 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>5-Set</t>
-  </si>
-  <si>
-    <t>9-Set</t>
+    <t>26-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>11-Set</t>
-  </si>
-  <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>12-Set</t>
-  </si>
-  <si>
-    <t>16-Set</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ambientes competitivos</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>18-Set</t>
-  </si>
-  <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
   </si>
   <si>
@@ -174,31 +162,16 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>19-Set</t>
-  </si>
-  <si>
-    <t>23-Set</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>25-Set</t>
-  </si>
-  <si>
-    <t>30-Set</t>
-  </si>
-  <si>
-    <t>2-Out</t>
-  </si>
-  <si>
     <t xml:space="preserve">Projeto Intermediário</t>
   </si>
   <si>
-    <t xml:space="preserve">Appling Coverage Path Planning Algorithms in Search and Rescue Operations</t>
+    <t xml:space="preserve">Tema a ser definido</t>
   </si>
   <si>
     <t xml:space="preserve"> Desenvolvimento de um agente autônomo que atua em um ambiente discreto, determinístico, síncrono, simulado e *single agent* ou *multi-agent*. </t>
@@ -207,16 +180,10 @@
     <t xml:space="preserve">Desenvolvimento de projeto em sala de aula</t>
   </si>
   <si>
-    <t>3-Out</t>
-  </si>
-  <si>
-    <t>7-Out</t>
-  </si>
-  <si>
-    <t>9-Out</t>
-  </si>
-  <si>
-    <t>14-Out</t>
+    <t>02-Abr</t>
+  </si>
+  <si>
+    <t>07-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Aprendendo políticas</t>
@@ -231,7 +198,7 @@
     <t xml:space="preserve"> Discussão em sala. Exercícios em sala de aula envolvendo o ambiente OpenAI Gym.  Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>16-Out</t>
+    <t>09-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Hiper-parâmetros do algoritmo Q-Learning</t>
@@ -246,7 +213,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>21-Out</t>
+    <t>14-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">SARSA: um exemplo de algoritmo on-policy</t>
@@ -261,7 +228,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>23-Out</t>
+    <t>16-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Trabalhando com ambientes não-determinísticos</t>
@@ -273,7 +240,10 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>28-Out</t>
+    <t>23-Abr</t>
+  </si>
+  <si>
+    <t>28-Abr</t>
   </si>
   <si>
     <t>Robótica</t>
@@ -285,7 +255,7 @@
     <t xml:space="preserve">Aula expositiva com discussão sobre o assunto.</t>
   </si>
   <si>
-    <t>30-Out</t>
+    <t>30-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
@@ -300,19 +270,19 @@
     <t xml:space="preserve">Desenvolvimento de projeto</t>
   </si>
   <si>
-    <t>4-Nov</t>
-  </si>
-  <si>
-    <t>6-Nov</t>
-  </si>
-  <si>
-    <t>11-Nov</t>
+    <t>05-Mai</t>
+  </si>
+  <si>
+    <t>07-Mai</t>
+  </si>
+  <si>
+    <t>12-Mai</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>13-Nov</t>
+    <t>14-Mai</t>
   </si>
 </sst>
 </file>
@@ -337,12 +307,24 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -357,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -380,10 +362,25 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,7 +894,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C14" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1091,8 +1088,8 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
+      <c r="A10" s="8">
+        <v>45726</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
@@ -1108,54 +1105,54 @@
         <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
+      <c r="A11" s="8">
+        <v>45728</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A12" s="8">
+        <v>45733</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="A13" s="9">
+        <v>45735</v>
+      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="3" t="s">
         <v>44</v>
       </c>
@@ -1171,360 +1168,305 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10">
+        <v>45740</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A15" s="10">
+        <v>45742</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A16" s="9">
+        <v>45747</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="C16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="49.5" customHeight="1">
       <c r="A17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="1"/>
+      <c r="E18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" ht="37.5" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" ht="36" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="1"/>
+      <c r="A20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>65</v>
+      <c r="A21" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="36" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>67</v>
+      <c r="A23" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="6"/>
+      <c r="A24" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="69" customHeight="1">
-      <c r="A25" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="3"/>
+      <c r="A25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A26" s="8" t="s">
-        <v>82</v>
+      <c r="A26" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" s="2" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A28" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" s="2" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>94</v>
+      <c r="B28" s="7"/>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="A29" s="4"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="A31" s="4"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="A32" s="4"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="G32" s="3"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">

</xml_diff>

<commit_message>
atualizacao do plano de aula e outras infos
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Data</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve"> Fundamentos / Conteúdo </t>
   </si>
   <si>
-    <t>Conteúdo</t>
+    <t>Dinâmica</t>
   </si>
   <si>
     <t xml:space="preserve"> Programação/Atividades </t>
@@ -120,9 +120,15 @@
     <t>26-Fev</t>
   </si>
   <si>
+    <t>10-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
+    <t>12-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
   </si>
   <si>
@@ -135,6 +141,9 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
+    <t>17-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ambientes competitivos</t>
   </si>
   <si>
@@ -150,6 +159,9 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
+    <t>19-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
   </si>
   <si>
@@ -162,10 +174,19 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
+    <t>24-Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>26-Mar</t>
+  </si>
+  <si>
+    <t>31-Mar</t>
   </si>
   <si>
     <t xml:space="preserve">Projeto Intermediário</t>
@@ -307,7 +328,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,12 +339,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="0"/>
         <bgColor theme="0" tint="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="5"/>
-        <bgColor indexed="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -339,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -350,10 +365,16 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -362,13 +383,13 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -377,10 +398,10 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -894,13 +915,14 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C14" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="2" style="1" width="19.147857142857141"/>
+    <col customWidth="1" min="1" max="1" style="1" width="29.140625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="19.147857142857141"/>
     <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="38.862142857142857"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="65.290714285714287"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="85.719285714285704"/>
@@ -930,7 +952,7 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -951,10 +973,10 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
@@ -970,10 +992,10 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" s="2" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -991,10 +1013,10 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1010,10 +1032,10 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1029,10 +1051,10 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1048,10 +1070,10 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1069,10 +1091,10 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1088,10 +1110,10 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="8">
-        <v>45726</v>
-      </c>
-      <c r="B10" s="7"/>
+      <c r="A10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1105,355 +1127,355 @@
         <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A11" s="8">
-        <v>45728</v>
+      <c r="A11" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="8">
-        <v>45733</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>39</v>
+      <c r="A12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A13" s="9">
-        <v>45735</v>
-      </c>
-      <c r="B13" s="7"/>
+      <c r="A13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="9"/>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A14" s="10">
-        <v>45740</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>49</v>
+      <c r="A14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A15" s="10">
-        <v>45742</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>49</v>
+      <c r="A15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A16" s="9">
-        <v>45747</v>
+      <c r="A16" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>54</v>
+      <c r="A17" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>56</v>
+      <c r="A18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" ht="37.5" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="6"/>
+      <c r="A19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" ht="36" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>65</v>
+      <c r="A20" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>70</v>
+      <c r="A21" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="36" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>74</v>
+      <c r="A22" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>76</v>
+      <c r="A23" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A24" s="12" t="s">
-        <v>79</v>
+      <c r="A24" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="69" customHeight="1">
-      <c r="A25" s="12" t="s">
-        <v>84</v>
+      <c r="A25" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A26" s="12" t="s">
-        <v>85</v>
+      <c r="A26" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A27" s="13" t="s">
-        <v>86</v>
+      <c r="A27" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>87</v>
+      <c r="C27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G27" s="3"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>87</v>
+      <c r="A28" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A29" s="4"/>
+      <c r="A29" s="7"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A30" s="4"/>
+      <c r="A30" s="7"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1461,17 +1483,17 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="4"/>
+      <c r="A31" s="7"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="9"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1479,8 +1501,8 @@
       <c r="G33" s="3"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1488,8 +1510,8 @@
       <c r="G34" s="3"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1497,26 +1519,26 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1524,8 +1546,8 @@
       <c r="G38" s="3"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1533,8 +1555,8 @@
       <c r="G39" s="3"/>
     </row>
     <row r="40" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1542,8 +1564,8 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -1551,8 +1573,8 @@
       <c r="G41" s="3"/>
     </row>
     <row r="42" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>

</xml_diff>

<commit_message>
alteracao do plano de aula para adicionar uma aula studio para o desenvolvimento do projeto intermediario
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Data</t>
   </si>
@@ -207,6 +207,12 @@
     <t>07-Abr</t>
   </si>
   <si>
+    <t>Studio</t>
+  </si>
+  <si>
+    <t>09-Abr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aprendendo políticas</t>
   </si>
   <si>
@@ -219,7 +225,7 @@
     <t xml:space="preserve"> Discussão em sala. Exercícios em sala de aula envolvendo o ambiente OpenAI Gym.  Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>09-Abr</t>
+    <t>14-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Hiper-parâmetros do algoritmo Q-Learning</t>
@@ -234,7 +240,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>14-Abr</t>
+    <t>16-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">SARSA: um exemplo de algoritmo on-policy</t>
@@ -249,7 +255,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>16-Abr</t>
+    <t>23-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Trabalhando com ambientes não-determinísticos</t>
@@ -261,12 +267,12 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>23-Abr</t>
-  </si>
-  <si>
     <t>28-Abr</t>
   </si>
   <si>
+    <t>30-Abr</t>
+  </si>
+  <si>
     <t>Robótica</t>
   </si>
   <si>
@@ -276,7 +282,7 @@
     <t xml:space="preserve">Aula expositiva com discussão sobre o assunto.</t>
   </si>
   <si>
-    <t>30-Abr</t>
+    <t>05-Mai</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
@@ -289,9 +295,6 @@
   </si>
   <si>
     <t xml:space="preserve">Desenvolvimento de projeto</t>
-  </si>
-  <si>
-    <t>05-Mai</t>
   </si>
   <si>
     <t>07-Mai</t>
@@ -354,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -395,13 +398,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1229,7 +1226,7 @@
       <c r="B16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1258,215 +1255,213 @@
       <c r="F17" s="1"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="13" t="s">
+    <row r="18" s="2" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" ht="37.5" customHeight="1">
-      <c r="A19" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" ht="37.5" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" ht="36" customHeight="1">
-      <c r="A20" s="13" t="s">
+      <c r="E20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" ht="36" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="E21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="36" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" ht="36" customHeight="1">
+      <c r="A23" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" s="2" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A23" s="14" t="s">
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="B24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A24" s="14" t="s">
+      <c r="C24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="69" customHeight="1">
-      <c r="A25" s="14" t="s">
+      <c r="E25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="F25" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A26" s="14" t="s">
-        <v>92</v>
+      <c r="A26" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A27" s="15" t="s">
-        <v>93</v>
+      <c r="A27" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G27" s="3"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A28" s="16" t="s">
-        <v>95</v>
+      <c r="A28" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G28" s="3"/>
     </row>

</xml_diff>

<commit_message>
primeira semana de aula 2025/2
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -36,7 +36,7 @@
     <t xml:space="preserve"> Programação/Atividades </t>
   </si>
   <si>
-    <t>03-Fev</t>
+    <t>11-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Inteligência Artificial</t>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referência: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>05-Fev</t>
+    <t>13-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">O que é agente autônomo? O que são propriedades de ambiente e como isto impacta o desenvolvimento de agentes autônomos? </t>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referências: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>10-Fev</t>
+    <t>18-Ago</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca cegos</t>
@@ -84,7 +84,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>12-Fev</t>
+    <t>20-Ago</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? </t>
@@ -96,13 +96,13 @@
     <t xml:space="preserve"> Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>17-Fev</t>
-  </si>
-  <si>
-    <t>19-Fev</t>
-  </si>
-  <si>
-    <t>24-Fev</t>
+    <t>01-Set</t>
+  </si>
+  <si>
+    <t>03-Set</t>
+  </si>
+  <si>
+    <t>04-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca informados</t>
@@ -117,16 +117,16 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>26-Fev</t>
-  </si>
-  <si>
-    <t>10-Mar</t>
+    <t>08-Set</t>
+  </si>
+  <si>
+    <t>10-Set</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>12-Mar</t>
+    <t>11-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>17-Mar</t>
+    <t>15-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Ambientes competitivos</t>
@@ -159,7 +159,7 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>19-Mar</t>
+    <t>17-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
@@ -174,7 +174,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>24-Mar</t>
+    <t>22-Set</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
@@ -183,10 +183,10 @@
     <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>26-Mar</t>
-  </si>
-  <si>
-    <t>31-Mar</t>
+    <t>24-Set</t>
+  </si>
+  <si>
+    <t>29-Set</t>
   </si>
   <si>
     <t xml:space="preserve">Projeto Intermediário</t>
@@ -201,16 +201,13 @@
     <t xml:space="preserve">Desenvolvimento de projeto em sala de aula</t>
   </si>
   <si>
-    <t>02-Abr</t>
-  </si>
-  <si>
-    <t>07-Abr</t>
-  </si>
-  <si>
-    <t>Studio</t>
-  </si>
-  <si>
-    <t>09-Abr</t>
+    <t>01-Out</t>
+  </si>
+  <si>
+    <t>06-Out</t>
+  </si>
+  <si>
+    <t>08-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Aprendendo políticas</t>
@@ -225,7 +222,7 @@
     <t xml:space="preserve"> Discussão em sala. Exercícios em sala de aula envolvendo o ambiente OpenAI Gym.  Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>14-Abr</t>
+    <t>13-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Hiper-parâmetros do algoritmo Q-Learning</t>
@@ -240,7 +237,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>16-Abr</t>
+    <t>15-Out</t>
   </si>
   <si>
     <t xml:space="preserve">SARSA: um exemplo de algoritmo on-policy</t>
@@ -255,7 +252,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>23-Abr</t>
+    <t>20-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Trabalhando com ambientes não-determinísticos</t>
@@ -267,10 +264,10 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>28-Abr</t>
-  </si>
-  <si>
-    <t>30-Abr</t>
+    <t>22-Out</t>
+  </si>
+  <si>
+    <t>27-Out</t>
   </si>
   <si>
     <t>Robótica</t>
@@ -282,7 +279,7 @@
     <t xml:space="preserve">Aula expositiva com discussão sobre o assunto.</t>
   </si>
   <si>
-    <t>05-Mai</t>
+    <t>29-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
@@ -297,16 +294,19 @@
     <t xml:space="preserve">Desenvolvimento de projeto</t>
   </si>
   <si>
-    <t>07-Mai</t>
-  </si>
-  <si>
-    <t>12-Mai</t>
+    <t>3-Nov</t>
+  </si>
+  <si>
+    <t>5-Nov</t>
+  </si>
+  <si>
+    <t>10-Nov</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>14-Mai</t>
+    <t>12-Nov</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -912,7 +912,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1256,15 +1256,15 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>63</v>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>60</v>
@@ -1273,20 +1273,20 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>51</v>
@@ -1294,163 +1294,163 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" ht="37.5" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>69</v>
+      <c r="A20" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" ht="36" customHeight="1">
+      <c r="A21" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="36" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" ht="36" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="60.75" customHeight="1">
       <c r="A24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="63" customHeight="1">
       <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A27" s="14" t="s">
+    <row r="27" s="2" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" s="2" customFormat="1" ht="57" customHeight="1">
+      <c r="A28" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" s="2" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="7" t="s">
         <v>95</v>
       </c>
@@ -1465,34 +1465,44 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A29" s="7"/>
+    <row r="29" s="2" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" s="2" customFormat="1" ht="57" customHeight="1">
+    <row r="30" s="2" customFormat="1" ht="48" customHeight="1">
       <c r="A30" s="7"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="31" s="2" customFormat="1" ht="57" customHeight="1">
       <c r="A31" s="7"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="7"/>
-      <c r="B32" s="9"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="9"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1504,22 +1514,22 @@
       <c r="F34" s="1"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
+    <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="36" s="2" customFormat="1" ht="39" customHeight="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1532,12 +1542,12 @@
       <c r="G37" s="3"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1576,6 +1586,15 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
+    <row r="43" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
material sobre q-learning, semana do dia 13/10
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -210,6 +210,9 @@
     <t>08-Out</t>
   </si>
   <si>
+    <t>13-Out</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aprendendo políticas</t>
   </si>
   <si>
@@ -222,7 +225,7 @@
     <t xml:space="preserve"> Discussão em sala. Exercícios em sala de aula envolvendo o ambiente OpenAI Gym.  Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>13-Out</t>
+    <t>15-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Hiper-parâmetros do algoritmo Q-Learning</t>
@@ -237,7 +240,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>15-Out</t>
+    <t>20-Out</t>
   </si>
   <si>
     <t xml:space="preserve">SARSA: um exemplo de algoritmo on-policy</t>
@@ -252,7 +255,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>20-Out</t>
+    <t>22-Out</t>
   </si>
   <si>
     <t xml:space="preserve">Trabalhando com ambientes não-determinísticos</t>
@@ -264,12 +267,12 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>22-Out</t>
-  </si>
-  <si>
     <t>27-Out</t>
   </si>
   <si>
+    <t>29-Out</t>
+  </si>
+  <si>
     <t>Robótica</t>
   </si>
   <si>
@@ -279,7 +282,7 @@
     <t xml:space="preserve">Aula expositiva com discussão sobre o assunto.</t>
   </si>
   <si>
-    <t>29-Out</t>
+    <t>3-Nov</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
@@ -292,9 +295,6 @@
   </si>
   <si>
     <t xml:space="preserve">Desenvolvimento de projeto</t>
-  </si>
-  <si>
-    <t>3-Nov</t>
   </si>
   <si>
     <t>5-Nov</t>
@@ -357,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -390,12 +390,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -912,7 +906,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1256,7 +1250,7 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="1"/>
@@ -1273,99 +1267,95 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" ht="37.5" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="E20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" ht="37.5" customHeight="1">
-      <c r="A20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="3" t="s">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" ht="36" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="F21" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" ht="36" customHeight="1">
       <c r="A22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" ht="36" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1373,57 +1363,58 @@
       <c r="A24" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="63" customHeight="1">
       <c r="A25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -1433,21 +1424,21 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G27" s="3"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="12" t="s">
         <v>94</v>
       </c>
       <c r="B28" s="1"/>

</xml_diff>

<commit_message>
tudo pronto para o inicio do semestre 2026.1
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Data</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve"> Programação/Atividades </t>
   </si>
   <si>
-    <t>11-Ago</t>
+    <t>09-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Inteligência Artificial</t>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referência: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>13-Ago</t>
+    <t>11-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">O que é agente autônomo? O que são propriedades de ambiente e como isto impacta o desenvolvimento de agentes autônomos? </t>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Dinâmica em grupo. Referências: Cap 1 e 2 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>18-Ago</t>
+    <t>23-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca cegos</t>
@@ -84,7 +84,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>20-Ago</t>
+    <t>25-Fev</t>
   </si>
   <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? </t>
@@ -96,13 +96,13 @@
     <t xml:space="preserve"> Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>01-Set</t>
-  </si>
-  <si>
-    <t>03-Set</t>
-  </si>
-  <si>
-    <t>04-Set</t>
+    <t>02-Mar</t>
+  </si>
+  <si>
+    <t>04-Mar</t>
+  </si>
+  <si>
+    <t>09-Mar</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos de busca informados</t>
@@ -117,16 +117,16 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>08-Set</t>
-  </si>
-  <si>
-    <t>10-Set</t>
+    <t>11-Mar</t>
+  </si>
+  <si>
+    <t>16-Mar</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>11-Set</t>
+    <t>18-Mar</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
@@ -141,7 +141,19 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>15-Set</t>
+    <t>23-Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>25-Mar</t>
+  </si>
+  <si>
+    <t>30-Mar</t>
   </si>
   <si>
     <t xml:space="preserve">Ambientes competitivos</t>
@@ -159,7 +171,7 @@
     <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>17-Set</t>
+    <t>01-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
@@ -174,19 +186,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>22-Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;SEMANA DE PROVAS - Prova Intermediária&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>24-Set</t>
-  </si>
-  <si>
-    <t>29-Set</t>
+    <t>06-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Projeto Intermediário</t>
@@ -201,16 +201,7 @@
     <t xml:space="preserve">Desenvolvimento de projeto em sala de aula</t>
   </si>
   <si>
-    <t>01-Out</t>
-  </si>
-  <si>
-    <t>06-Out</t>
-  </si>
-  <si>
-    <t>08-Out</t>
-  </si>
-  <si>
-    <t>13-Out</t>
+    <t>08-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Aprendendo políticas</t>
@@ -225,7 +216,7 @@
     <t xml:space="preserve"> Discussão em sala. Exercícios em sala de aula envolvendo o ambiente OpenAI Gym.  Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>15-Out</t>
+    <t>13-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Hiper-parâmetros do algoritmo Q-Learning</t>
@@ -240,7 +231,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>20-Out</t>
+    <t>15-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">SARSA: um exemplo de algoritmo on-policy</t>
@@ -255,7 +246,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>22-Out</t>
+    <t>22-Abr</t>
   </si>
   <si>
     <t xml:space="preserve">Trabalhando com ambientes não-determinísticos</t>
@@ -267,10 +258,10 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning e Sarsa</t>
   </si>
   <si>
-    <t>27-Out</t>
-  </si>
-  <si>
-    <t>29-Out</t>
+    <t>27-Abr</t>
+  </si>
+  <si>
+    <t>29-Abr</t>
   </si>
   <si>
     <t>Robótica</t>
@@ -282,7 +273,7 @@
     <t xml:space="preserve">Aula expositiva com discussão sobre o assunto.</t>
   </si>
   <si>
-    <t>3-Nov</t>
+    <t>04-Mai</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para desenvolver um agente robótico? </t>
@@ -297,16 +288,16 @@
     <t xml:space="preserve">Desenvolvimento de projeto</t>
   </si>
   <si>
-    <t>5-Nov</t>
-  </si>
-  <si>
-    <t>10-Nov</t>
+    <t>06-Mai</t>
+  </si>
+  <si>
+    <t>11-Mai</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Avaliação Final da disciplina&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>12-Nov</t>
+    <t>13-Mai</t>
   </si>
 </sst>
 </file>
@@ -357,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -389,10 +380,13 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -906,7 +900,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1141,80 +1135,79 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="63" customHeight="1">
       <c r="A13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="63" customHeight="1">
       <c r="A15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+    <row r="16" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1232,291 +1225,242 @@
       <c r="F16" s="1"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" s="2" customFormat="1" ht="49.5" customHeight="1">
+    <row r="17" s="2" customFormat="1" ht="63" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="1"/>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" s="2" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="1"/>
+    <row r="18" s="2" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" ht="37.5" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>65</v>
-      </c>
+    <row r="19" s="2" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" s="2" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" ht="36" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>75</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" ht="36" customHeight="1">
-      <c r="A22" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="3"/>
+    <row r="22" ht="37.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" ht="36" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>79</v>
+      <c r="A23" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" s="2" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>83</v>
+    <row r="24" ht="36" customHeight="1">
+      <c r="A24" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="63" customHeight="1">
-      <c r="A25" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" ht="36" customHeight="1">
+      <c r="A25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="D25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" s="2" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A26" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" s="2" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>92</v>
-      </c>
+    <row r="27" s="2" customFormat="1" ht="63" customHeight="1">
+      <c r="A27" s="12"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>95</v>
-      </c>
+    <row r="28" s="2" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" s="2" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A29" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>95</v>
-      </c>
+    <row r="29" s="2" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A29" s="11"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A30" s="7"/>
+    <row r="30" s="2" customFormat="1" ht="57" customHeight="1">
       <c r="G30" s="3"/>
     </row>
-    <row r="31" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+    <row r="31" s="2" customFormat="1" ht="59.25" customHeight="1">
       <c r="G31" s="3"/>
     </row>
-    <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="32" s="2" customFormat="1" ht="48" customHeight="1">
       <c r="A32" s="7"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="33" s="2" customFormat="1" ht="57" customHeight="1">
       <c r="A33" s="7"/>
-      <c r="B33" s="9"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="7"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="9"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
+    <row r="36" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1524,39 +1468,39 @@
       <c r="G36" s="3"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="38" s="2" customFormat="1" ht="39" customHeight="1">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1586,6 +1530,24 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
+    <row r="44" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>